<commit_message>
update valueset references in IG
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-Claim.xlsx
+++ b/v0.7/StructureDefinition-Claim.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5187" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5187" uniqueCount="688">
   <si>
     <t>Property</t>
   </si>
@@ -1085,7 +1085,7 @@
     <t>The role codes for the care team members.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/claim-careteamrole</t>
+    <t>https://ig.hcxprotocol.io/v0.7/ValueSet-health-service-provider-role.html</t>
   </si>
   <si>
     <t>Claim.careTeam.qualification</t>
@@ -1103,7 +1103,7 @@
     <t>Provider professional qualifications.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/provider-qualification</t>
+    <t>https://ig.hcxprotocol.io/v0.7/ValueSet-medical-speciality-type-provider.html</t>
   </si>
   <si>
     <t>Claim.supportingInfo</t>
@@ -1170,7 +1170,7 @@
     <t>The valuset used for additional information category codes.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/claim-informationcategory</t>
+    <t>https://ig.hcxprotocol.io/v0.7/ValueSet-claim-supporting-info-categories.html</t>
   </si>
   <si>
     <t>Claim.supportingInfo.code</t>
@@ -1188,7 +1188,7 @@
     <t>The valuset used for additional information codes.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/claim-exception</t>
+    <t>https://ig.hcxprotocol.io/v0.7/ValueSet-claim-supporting-info-codes.html</t>
   </si>
   <si>
     <t>Claim.supportingInfo.timing[x]</t>
@@ -1785,7 +1785,7 @@
     <t>Benefit categories such as: oral-basic, major, glasses.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/ex-benefitcategory</t>
+    <t>https://ig.hcxprotocol.io/v0.7/ValueSet-claim-service-categories.html</t>
   </si>
   <si>
     <t>Claim.item.productOrService</t>
@@ -2040,6 +2040,9 @@
     <t>Claim.item.detail.category</t>
   </si>
   <si>
+    <t>https://ig.hcxprotocol.io/v0.7/ValueSet-billing-subgroup-categories.html</t>
+  </si>
+  <si>
     <t>Claim.item.detail.productOrService</t>
   </si>
   <si>
@@ -2089,6 +2092,9 @@
   </si>
   <si>
     <t>Claim.item.detail.subDetail.category</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/ex-benefitcategory</t>
   </si>
   <si>
     <t>Claim.item.detail.subDetail.productOrService</t>
@@ -2454,7 +2460,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.9609375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="120.6484375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="52.37109375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.84375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="18.84765625" customWidth="true" bestFit="true"/>
@@ -16118,7 +16124,7 @@
         <v>573</v>
       </c>
       <c r="Y126" t="s" s="2">
-        <v>574</v>
+        <v>657</v>
       </c>
       <c r="Z126" t="s" s="2">
         <v>75</v>
@@ -16162,7 +16168,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -16246,7 +16252,7 @@
         <v>75</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>81</v>
@@ -16272,7 +16278,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -16298,13 +16304,13 @@
         <v>157</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L128" t="s" s="2">
         <v>585</v>
       </c>
       <c r="M128" t="s" s="2">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="N128" t="s" s="2">
         <v>587</v>
@@ -16356,7 +16362,7 @@
         <v>75</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>73</v>
@@ -16382,7 +16388,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -16466,7 +16472,7 @@
         <v>75</v>
       </c>
       <c r="AE129" t="s" s="2">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="AF129" t="s" s="2">
         <v>73</v>
@@ -16492,7 +16498,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
@@ -16574,7 +16580,7 @@
         <v>75</v>
       </c>
       <c r="AE130" t="s" s="2">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="AF130" t="s" s="2">
         <v>73</v>
@@ -16600,7 +16606,7 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -16682,7 +16688,7 @@
         <v>75</v>
       </c>
       <c r="AE131" t="s" s="2">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="AF131" t="s" s="2">
         <v>73</v>
@@ -16708,7 +16714,7 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -16792,7 +16798,7 @@
         <v>75</v>
       </c>
       <c r="AE132" t="s" s="2">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="AF132" t="s" s="2">
         <v>73</v>
@@ -16818,7 +16824,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" t="s" s="2">
@@ -16902,7 +16908,7 @@
         <v>75</v>
       </c>
       <c r="AE133" t="s" s="2">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="AF133" t="s" s="2">
         <v>73</v>
@@ -16928,7 +16934,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
@@ -17010,7 +17016,7 @@
         <v>75</v>
       </c>
       <c r="AE134" t="s" s="2">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="AF134" t="s" s="2">
         <v>73</v>
@@ -17036,7 +17042,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
@@ -17118,7 +17124,7 @@
         <v>75</v>
       </c>
       <c r="AE135" t="s" s="2">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="AF135" t="s" s="2">
         <v>73</v>
@@ -17144,7 +17150,7 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
@@ -17250,7 +17256,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="2">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" t="s" s="2">
@@ -17358,7 +17364,7 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" t="s" s="2">
@@ -17468,7 +17474,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="2">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
@@ -17550,7 +17556,7 @@
         <v>75</v>
       </c>
       <c r="AE139" t="s" s="2">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="AF139" t="s" s="2">
         <v>81</v>
@@ -17576,7 +17582,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="2">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
@@ -17658,7 +17664,7 @@
         <v>75</v>
       </c>
       <c r="AE140" t="s" s="2">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="AF140" t="s" s="2">
         <v>73</v>
@@ -17684,7 +17690,7 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="2">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
@@ -17750,7 +17756,7 @@
         <v>573</v>
       </c>
       <c r="Y141" t="s" s="2">
-        <v>574</v>
+        <v>675</v>
       </c>
       <c r="Z141" t="s" s="2">
         <v>75</v>
@@ -17768,7 +17774,7 @@
         <v>75</v>
       </c>
       <c r="AE141" t="s" s="2">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="AF141" t="s" s="2">
         <v>73</v>
@@ -17794,7 +17800,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="2">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -17878,7 +17884,7 @@
         <v>75</v>
       </c>
       <c r="AE142" t="s" s="2">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="AF142" t="s" s="2">
         <v>81</v>
@@ -17904,7 +17910,7 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="2">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -17930,13 +17936,13 @@
         <v>157</v>
       </c>
       <c r="K143" t="s" s="2">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L143" t="s" s="2">
         <v>585</v>
       </c>
       <c r="M143" t="s" s="2">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="N143" t="s" s="2">
         <v>587</v>
@@ -17988,7 +17994,7 @@
         <v>75</v>
       </c>
       <c r="AE143" t="s" s="2">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="AF143" t="s" s="2">
         <v>73</v>
@@ -18014,7 +18020,7 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="2">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -18098,7 +18104,7 @@
         <v>75</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>73</v>
@@ -18124,7 +18130,7 @@
     </row>
     <row r="145">
       <c r="A145" t="s" s="2">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -18206,7 +18212,7 @@
         <v>75</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>73</v>
@@ -18232,7 +18238,7 @@
     </row>
     <row r="146">
       <c r="A146" t="s" s="2">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -18314,7 +18320,7 @@
         <v>75</v>
       </c>
       <c r="AE146" t="s" s="2">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="AF146" t="s" s="2">
         <v>73</v>
@@ -18340,7 +18346,7 @@
     </row>
     <row r="147">
       <c r="A147" t="s" s="2">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -18424,7 +18430,7 @@
         <v>75</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>73</v>
@@ -18450,7 +18456,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s" s="2">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -18534,7 +18540,7 @@
         <v>75</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>73</v>
@@ -18560,7 +18566,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" t="s" s="2">
@@ -18642,7 +18648,7 @@
         <v>75</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>73</v>
@@ -18668,7 +18674,7 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="2">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
@@ -18694,14 +18700,14 @@
         <v>614</v>
       </c>
       <c r="K150" t="s" s="2">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="M150" s="2"/>
       <c r="N150" t="s" s="2">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="O150" t="s" s="2">
         <v>75</v>
@@ -18750,7 +18756,7 @@
         <v>75</v>
       </c>
       <c r="AE150" t="s" s="2">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="AF150" t="s" s="2">
         <v>73</v>

</xml_diff>

<commit_message>
update careteam role & qualification value sets
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-Claim.xlsx
+++ b/v0.7/StructureDefinition-Claim.xlsx
@@ -1085,7 +1085,7 @@
     <t>The role codes for the care team members.</t>
   </si>
   <si>
-    <t>https://ig.hcxprotocol.io/v0.7/ValueSet-health-service-provider-role.html</t>
+    <t>https://nrces.in/ndhm/fhir/r4/ValueSet-ndhm-practitioner-role.html</t>
   </si>
   <si>
     <t>Claim.careTeam.qualification</t>
@@ -1094,10 +1094,10 @@
     <t>Practitioner credential or specialization</t>
   </si>
   <si>
-    <t>The qualification of the practitioner which is applicable for this service.</t>
-  </si>
-  <si>
-    <t>Need to specify which qualification a provider is delivering the product or service under.</t>
+    <t>The specialization of the practitioner or provider which is applicable for this service. The use case for the speciality here is to validate the diagnosis and procedure and check its relevance.</t>
+  </si>
+  <si>
+    <t>Need to specify which specialization a practitioner or provider acting under when delivering the product or service.</t>
   </si>
   <si>
     <t>Provider professional qualifications.</t>

</xml_diff>